<commit_message>
product completed. test cases modified.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/product_modify_test_cases.xlsx
+++ b/soberano/test_cases/product_modify_test_cases.xlsx
@@ -365,7 +365,7 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="12:12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -844,7 +844,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>58</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>60</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>62</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>63</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>64</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>65</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>66</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>67</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>68</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>69</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>70</v>

</xml_diff>